<commit_message>
adicionando confirmação de atualização
</commit_message>
<xml_diff>
--- a/output/processos_extraidos.xlsx
+++ b/output/processos_extraidos.xlsx
@@ -456,7 +456,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="17" customWidth="1" min="1" max="1"/>
     <col width="29" customWidth="1" min="2" max="2"/>
     <col width="27" customWidth="1" min="3" max="3"/>
     <col width="27" customWidth="1" min="4" max="4"/>
@@ -499,7 +499,7 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>processo_2</t>
+          <t>copy_processo_2</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
@@ -547,10 +547,8 @@
           <t>Advogado Exemplo</t>
         </is>
       </c>
-      <c r="E3" s="3" t="inlineStr">
-        <is>
-          <t>44432</t>
-        </is>
+      <c r="E3" s="3" t="n">
+        <v>44432</v>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
corrigindo confirmação de atualização
</commit_message>
<xml_diff>
--- a/output/processos_extraidos.xlsx
+++ b/output/processos_extraidos.xlsx
@@ -499,17 +499,17 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>copy_processo_2</t>
+          <t>copy_processo_1</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>4835245-15.2024.8.01.2832</t>
+          <t>3781128-20.2024.8.01.8252</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>Nome Aleatório 2</t>
+          <t>Nome Aleatório 86</t>
         </is>
       </c>
       <c r="D2" s="3" t="inlineStr">
@@ -518,28 +518,28 @@
         </is>
       </c>
       <c r="E2" s="3" t="n">
-        <v>12723</v>
+        <v>44432</v>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>25/5/2024</t>
+          <t>12/5/2024</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>processo_1</t>
+          <t>copy_processo_2</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>3781128-20.2024.8.01.8252</t>
+          <t>4835245-15.2024.8.01.2832</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>Nome Aleatório 86</t>
+          <t>Nome Aleatório 2</t>
         </is>
       </c>
       <c r="D3" s="3" t="inlineStr">
@@ -547,12 +547,14 @@
           <t>Advogado Exemplo</t>
         </is>
       </c>
-      <c r="E3" s="3" t="n">
-        <v>44432</v>
+      <c r="E3" s="3" t="inlineStr">
+        <is>
+          <t>12723</t>
+        </is>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>12/5/2024</t>
+          <t>25/5/2024</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
corrigindo o padrão de data
Adicionando um padrão de data mais abrangente
</commit_message>
<xml_diff>
--- a/output/processos_extraidos.xlsx
+++ b/output/processos_extraidos.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -529,30 +529,60 @@
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>copy_processo_2</t>
+          <t>copy_processo_3</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
+          <t>3130687-11.2024.8.01.5042</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>Nome Aleatório 98</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t>Advogado Exemplo</t>
+        </is>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>43679</v>
+      </c>
+      <c r="F3" s="3" t="inlineStr">
+        <is>
+          <t>7/8/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>processo_2</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
           <t>4835245-15.2024.8.01.2832</t>
         </is>
       </c>
-      <c r="C3" s="3" t="inlineStr">
+      <c r="C4" s="3" t="inlineStr">
         <is>
           <t>Nome Aleatório 2</t>
         </is>
       </c>
-      <c r="D3" s="3" t="inlineStr">
+      <c r="D4" s="3" t="inlineStr">
         <is>
           <t>Advogado Exemplo</t>
         </is>
       </c>
-      <c r="E3" s="3" t="inlineStr">
+      <c r="E4" s="3" t="inlineStr">
         <is>
           <t>12723</t>
         </is>
       </c>
-      <c r="F3" s="3" t="inlineStr">
+      <c r="F4" s="3" t="inlineStr">
         <is>
           <t>25/5/2024</t>
         </is>

</xml_diff>

<commit_message>
tratando erro de formato de arquivo
</commit_message>
<xml_diff>
--- a/output/processos_extraidos.xlsx
+++ b/output/processos_extraidos.xlsx
@@ -456,7 +456,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="17" customWidth="1" min="1" max="1"/>
+    <col width="22" customWidth="1" min="1" max="1"/>
     <col width="29" customWidth="1" min="2" max="2"/>
     <col width="27" customWidth="1" min="3" max="3"/>
     <col width="27" customWidth="1" min="4" max="4"/>
@@ -499,17 +499,17 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>copy_processo_1</t>
+          <t>processo_2</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>3781128-20.2024.8.01.8252</t>
+          <t>4835245-15.2024.8.01.2832</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>Nome Aleatório 86</t>
+          <t>Nome Aleatório 2</t>
         </is>
       </c>
       <c r="D2" s="3" t="inlineStr">
@@ -518,28 +518,28 @@
         </is>
       </c>
       <c r="E2" s="3" t="n">
-        <v>44432</v>
+        <v>12723</v>
       </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>12/5/2024</t>
+          <t>25/5/2024</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>processo_2</t>
+          <t>processo_word</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>4835245-15.2024.8.01.2832</t>
+          <t>3781128-20.2024.8.01.8252</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>Nome Aleatório 2</t>
+          <t>Nome Aleatório 86</t>
         </is>
       </c>
       <c r="D3" s="3" t="inlineStr">
@@ -547,14 +547,12 @@
           <t>Advogado Exemplo</t>
         </is>
       </c>
-      <c r="E3" s="3" t="inlineStr">
-        <is>
-          <t>12723</t>
-        </is>
+      <c r="E3" s="3" t="n">
+        <v>44432</v>
       </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>25/5/2024</t>
+          <t>12/5/2024</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
adicionando uma interface gráfica simples
</commit_message>
<xml_diff>
--- a/output/processos_extraidos.xlsx
+++ b/output/processos_extraidos.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -28,30 +28,13 @@
     <font>
       <b val="1"/>
     </font>
-    <font>
-      <b val="1"/>
-      <color rgb="00FFFFFF"/>
-      <sz val="12"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="0016365c"/>
-        <bgColor rgb="004F81BD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00b8d9ff"/>
-        <bgColor rgb="00b8d9ff"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -72,16 +55,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -448,113 +425,75 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="22" customWidth="1" min="1" max="1"/>
-    <col width="29" customWidth="1" min="2" max="2"/>
-    <col width="27" customWidth="1" min="3" max="3"/>
-    <col width="27" customWidth="1" min="4" max="4"/>
-    <col width="12" customWidth="1" min="5" max="5"/>
-    <col width="22" customWidth="1" min="6" max="6"/>
-  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Arquivo</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Número do Processo</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Autor</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Advogado</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>OAB</t>
         </is>
       </c>
-      <c r="F1" s="2" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Data de Distribuição</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="inlineStr">
-        <is>
-          <t>processo_1</t>
-        </is>
-      </c>
-      <c r="B2" s="3" t="inlineStr">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>copy_processo_1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>3781128-20.2024.8.01.8252</t>
         </is>
       </c>
-      <c r="C2" s="3" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>Nome Aleatório 86</t>
         </is>
       </c>
-      <c r="D2" s="3" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>Advogado Exemplo</t>
         </is>
       </c>
-      <c r="E2" s="3" t="n">
-        <v>44432</v>
-      </c>
-      <c r="F2" s="3" t="inlineStr">
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>44432</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
         <is>
           <t>12/5/2024</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="inlineStr">
-        <is>
-          <t>processo_4</t>
-        </is>
-      </c>
-      <c r="B3" s="3" t="inlineStr">
-        <is>
-          <t>8719362-62.2024.8.12.0001</t>
-        </is>
-      </c>
-      <c r="C3" s="3" t="inlineStr">
-        <is>
-          <t>João da Silva</t>
-        </is>
-      </c>
-      <c r="D3" s="3" t="inlineStr">
-        <is>
-          <t>Maria Souza</t>
-        </is>
-      </c>
-      <c r="E3" s="3" t="inlineStr">
-        <is>
-          <t>10468</t>
-        </is>
-      </c>
-      <c r="F3" s="3" t="inlineStr">
-        <is>
-          <t>24/01/2024</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
melhorando a interface 1.1
</commit_message>
<xml_diff>
--- a/output/processos_extraidos.xlsx
+++ b/output/processos_extraidos.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,7 +459,7 @@
     <col width="22" customWidth="1" min="1" max="1"/>
     <col width="29" customWidth="1" min="2" max="2"/>
     <col width="27" customWidth="1" min="3" max="3"/>
-    <col width="27" customWidth="1" min="4" max="4"/>
+    <col width="59" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
     <col width="22" customWidth="1" min="6" max="6"/>
   </cols>
@@ -499,12 +499,12 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>processo_adv</t>
+          <t>processo_adv_oab</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>1855099-63.2024.8.12.0001</t>
+          <t>3286875-61.2024.8.12.0001</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
@@ -513,53 +513,57 @@
         </is>
       </c>
       <c r="D2" s="3" t="n"/>
-      <c r="E2" s="3" t="n">
-        <v>45950</v>
-      </c>
+      <c r="E2" s="3" t="n"/>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>16/08/2024</t>
+          <t>9/02/2024</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>processo_adv_oab</t>
+          <t>processo_3</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>3286875-61.2024.8.12.0001</t>
+          <t>3130687-11.2024.8.01.5042</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>João da Silva</t>
-        </is>
-      </c>
-      <c r="D3" s="3" t="n"/>
-      <c r="E3" s="3" t="n"/>
+          <t>Nome Aleatório 98</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Advogado Exemplo </t>
+        </is>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>43679</v>
+      </c>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>9/02/2024</t>
+          <t>7/8/2024</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>processo_2</t>
+          <t>processo_1</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>4835245-15.2024.8.01.2832</t>
+          <t>3781128-20.2024.8.01.8252</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>Nome Aleatório 2</t>
+          <t>Nome Aleatório 86</t>
         </is>
       </c>
       <c r="D4" s="3" t="inlineStr">
@@ -568,43 +572,102 @@
         </is>
       </c>
       <c r="E4" s="3" t="n">
-        <v>12723</v>
+        <v>44432</v>
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
-          <t>25/5/2024</t>
+          <t>12/5/2024</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>processo_1</t>
+          <t>processo_4</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>3781128-20.2024.8.01.8252</t>
+          <t>8719362-62.2024.8.12.0001</t>
         </is>
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>Nome Aleatório 86</t>
+          <t>João da Silva</t>
         </is>
       </c>
       <c r="D5" s="3" t="inlineStr">
         <is>
+          <t xml:space="preserve">Maria Souza
+OAB: 10468
+Data de Distribuição: 24/01/2024
+</t>
+        </is>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>10468</v>
+      </c>
+      <c r="F5" s="3" t="inlineStr">
+        <is>
+          <t>24/01/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>processo_2</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>4835245-15.2024.8.01.2832</t>
+        </is>
+      </c>
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>Nome Aleatório 2</t>
+        </is>
+      </c>
+      <c r="D6" s="3" t="inlineStr">
+        <is>
           <t xml:space="preserve">Advogado Exemplo </t>
         </is>
       </c>
-      <c r="E5" s="3" t="inlineStr">
-        <is>
-          <t>44432</t>
-        </is>
-      </c>
-      <c r="F5" s="3" t="inlineStr">
-        <is>
-          <t>12/5/2024</t>
+      <c r="E6" s="3" t="n">
+        <v>12723</v>
+      </c>
+      <c r="F6" s="3" t="inlineStr">
+        <is>
+          <t>25/5/2024</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="inlineStr">
+        <is>
+          <t>processo_adv</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>1855099-63.2024.8.12.0001</t>
+        </is>
+      </c>
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>João da Silva</t>
+        </is>
+      </c>
+      <c r="D7" s="3" t="n"/>
+      <c r="E7" s="3" t="inlineStr">
+        <is>
+          <t>45950</t>
+        </is>
+      </c>
+      <c r="F7" s="3" t="inlineStr">
+        <is>
+          <t>16/08/2024</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
adicionando o arquivo excel dinamico e animação
</commit_message>
<xml_diff>
--- a/output/processos_extraidos.xlsx
+++ b/output/processos_extraidos.xlsx
@@ -448,7 +448,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,7 +459,7 @@
     <col width="22" customWidth="1" min="1" max="1"/>
     <col width="29" customWidth="1" min="2" max="2"/>
     <col width="27" customWidth="1" min="3" max="3"/>
-    <col width="59" customWidth="1" min="4" max="4"/>
+    <col width="48" customWidth="1" min="4" max="4"/>
     <col width="12" customWidth="1" min="5" max="5"/>
     <col width="22" customWidth="1" min="6" max="6"/>
   </cols>
@@ -499,124 +499,123 @@
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
         <is>
-          <t>processo_adv_oab</t>
+          <t>processo_3</t>
         </is>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>3286875-61.2024.8.12.0001</t>
+          <t>3130687-11.2024.8.01.5042</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>João da Silva</t>
-        </is>
-      </c>
-      <c r="D2" s="3" t="n"/>
-      <c r="E2" s="3" t="n"/>
+          <t>Nome Aleatório 98</t>
+        </is>
+      </c>
+      <c r="D2" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Advogado Exemplo </t>
+        </is>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>43679</v>
+      </c>
       <c r="F2" s="3" t="inlineStr">
         <is>
-          <t>9/02/2024</t>
+          <t>7/8/2024</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
         <is>
-          <t>processo_3</t>
+          <t>processo_oab</t>
         </is>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>3130687-11.2024.8.01.5042</t>
+          <t>5056353-90.2024.8.12.0001</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>Nome Aleatório 98</t>
+          <t>João da Silva</t>
         </is>
       </c>
       <c r="D3" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Advogado Exemplo </t>
-        </is>
-      </c>
-      <c r="E3" s="3" t="n">
-        <v>43679</v>
-      </c>
+          <t xml:space="preserve">Maria Souza
+Data de Distribuição: 18/04/2024
+</t>
+        </is>
+      </c>
+      <c r="E3" s="3" t="n"/>
       <c r="F3" s="3" t="inlineStr">
         <is>
-          <t>7/8/2024</t>
+          <t>18/04/2024</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>processo_1</t>
+          <t>processo_adv</t>
         </is>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>3781128-20.2024.8.01.8252</t>
+          <t>1855099-63.2024.8.12.0001</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>Nome Aleatório 86</t>
-        </is>
-      </c>
-      <c r="D4" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Advogado Exemplo </t>
-        </is>
-      </c>
+          <t>João da Silva</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="n"/>
       <c r="E4" s="3" t="n">
-        <v>44432</v>
+        <v>45950</v>
       </c>
       <c r="F4" s="3" t="inlineStr">
         <is>
-          <t>12/5/2024</t>
+          <t>16/08/2024</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>processo_4</t>
+          <t>processo_1</t>
         </is>
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>8719362-62.2024.8.12.0001</t>
+          <t>3781128-20.2024.8.01.8252</t>
         </is>
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>João da Silva</t>
+          <t>Nome Aleatório 86</t>
         </is>
       </c>
       <c r="D5" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Maria Souza
-OAB: 10468
-Data de Distribuição: 24/01/2024
-</t>
+          <t xml:space="preserve">Advogado Exemplo </t>
         </is>
       </c>
       <c r="E5" s="3" t="n">
-        <v>10468</v>
+        <v>44432</v>
       </c>
       <c r="F5" s="3" t="inlineStr">
         <is>
-          <t>24/01/2024</t>
+          <t>12/5/2024</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>processo_2</t>
+          <t>copy_processo_2</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
@@ -634,40 +633,14 @@
           <t xml:space="preserve">Advogado Exemplo </t>
         </is>
       </c>
-      <c r="E6" s="3" t="n">
-        <v>12723</v>
+      <c r="E6" s="3" t="inlineStr">
+        <is>
+          <t>12723</t>
+        </is>
       </c>
       <c r="F6" s="3" t="inlineStr">
         <is>
           <t>25/5/2024</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="3" t="inlineStr">
-        <is>
-          <t>processo_adv</t>
-        </is>
-      </c>
-      <c r="B7" s="3" t="inlineStr">
-        <is>
-          <t>1855099-63.2024.8.12.0001</t>
-        </is>
-      </c>
-      <c r="C7" s="3" t="inlineStr">
-        <is>
-          <t>João da Silva</t>
-        </is>
-      </c>
-      <c r="D7" s="3" t="n"/>
-      <c r="E7" s="3" t="inlineStr">
-        <is>
-          <t>45950</t>
-        </is>
-      </c>
-      <c r="F7" s="3" t="inlineStr">
-        <is>
-          <t>16/08/2024</t>
         </is>
       </c>
     </row>

</xml_diff>